<commit_message>
Better code reuse and handling of setting the current value
</commit_message>
<xml_diff>
--- a/extras/sample-form/slider-label-buttons-sample.xlsx
+++ b/extras/sample-form/slider-label-buttons-sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdimeo\Code\cof\slider-label-extra-buttons\extras\sample-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A5A6CA-9B26-4654-9E68-FD8FFF781B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD792E02-B0C4-4B1E-B534-6EC0C810465E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="1920" windowWidth="23250" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2980,14 +2980,14 @@
     <t>custom_value7</t>
   </si>
   <si>
+    <t>&lt;p&gt;&lt;strong&gt;Slider with labels and extra buttons&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&lt;code&gt;custom-slider-label-buttons(min="0", max="1", markers="labels", step=0.25, button1="I don't know", value1=-99)&lt;/code&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>custom-slider-label-buttons(min="0", max="1", markers="labels", step=0.25, button1="I don't know", value1=-99)</t>
+  </si>
+  <si>
     <t>Value 7 = ${custom_value7}</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Slider with labels and extra buttons&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;&lt;code&gt;custom-slider-label-buttons(min="0", max="1", markers="labels", step=0.25, display_value='no', button1="I don't know", value1=-99)&lt;/code&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>custom-slider-label-buttons(min="0", max="1", markers="labels", step=0.25, display_value='no', button1="I don't know", value1=-99)</t>
   </si>
 </sst>
 </file>
@@ -4721,7 +4721,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4980,10 +4980,10 @@
         <v>372</v>
       </c>
       <c r="C13" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="F13" s="43" t="s">
         <v>374</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -4999,7 +4999,7 @@
         <v>369</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5259,7 @@
       </c>
       <c r="C2" s="6" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2203152337</v>
+        <v>2203160955</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>

</xml_diff>